<commit_message>
Matriz predictiva corregida y revisada
</commit_message>
<xml_diff>
--- a/docs/matriz-tokensAngel.xlsx
+++ b/docs/matriz-tokensAngel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jose\Documents\GitHub\compiler-intepreter\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jose\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="196">
   <si>
     <t>l</t>
   </si>
@@ -601,19 +601,38 @@
   </si>
   <si>
     <t>FACT</t>
+  </si>
+  <si>
+    <t>3, 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7   5</t>
+  </si>
+  <si>
+    <t>51    52</t>
+  </si>
+  <si>
+    <t>56   600</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -712,8 +731,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -797,6 +822,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -835,50 +872,50 @@
   </borders>
   <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -887,55 +924,73 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="35" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="35"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="35" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="35" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="35"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="35" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="35" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="35" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="35" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="1" xfId="36" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="35" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="35" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="1" xfId="36" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="35" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="35" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="35" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="35" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="35" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="35" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="1" xfId="35" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="37">
@@ -3869,9 +3924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4092,7 +4145,7 @@
       <c r="X2" s="32">
         <v>600</v>
       </c>
-      <c r="Y2" s="32">
+      <c r="Y2" s="36">
         <v>0</v>
       </c>
       <c r="Z2" s="32">
@@ -4172,7 +4225,7 @@
       <c r="B3" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="36">
         <v>2</v>
       </c>
       <c r="D3" s="32">
@@ -4244,7 +4297,7 @@
       <c r="Z3" s="36">
         <v>2</v>
       </c>
-      <c r="AA3" s="32">
+      <c r="AA3" s="36">
         <v>1</v>
       </c>
       <c r="AB3" s="32">
@@ -4277,34 +4330,34 @@
       <c r="AK3" s="32">
         <v>600</v>
       </c>
-      <c r="AL3" s="32">
+      <c r="AL3" s="36">
         <v>2</v>
       </c>
-      <c r="AM3" s="32">
+      <c r="AM3" s="36">
         <v>2</v>
       </c>
-      <c r="AN3" s="32">
+      <c r="AN3" s="36">
         <v>2</v>
       </c>
-      <c r="AO3" s="32">
+      <c r="AO3" s="36">
         <v>2</v>
       </c>
-      <c r="AP3" s="32">
+      <c r="AP3" s="36">
         <v>2</v>
       </c>
-      <c r="AQ3" s="32">
+      <c r="AQ3" s="36">
         <v>2</v>
       </c>
-      <c r="AR3" s="32">
+      <c r="AR3" s="36">
         <v>2</v>
       </c>
       <c r="AS3" s="32">
         <v>600</v>
       </c>
-      <c r="AT3" s="32">
+      <c r="AT3" s="36">
         <v>2</v>
       </c>
-      <c r="AU3" s="32">
+      <c r="AU3" s="36">
         <v>2</v>
       </c>
       <c r="AV3" s="32">
@@ -4318,8 +4371,8 @@
       <c r="B4" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="C4" s="32">
-        <v>3</v>
+      <c r="C4" s="41" t="s">
+        <v>192</v>
       </c>
       <c r="D4" s="32">
         <v>600</v>
@@ -4464,7 +4517,7 @@
       <c r="B5" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="36">
         <v>4</v>
       </c>
       <c r="D5" s="32">
@@ -4610,7 +4663,7 @@
       <c r="B6" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="36">
         <v>79</v>
       </c>
       <c r="D6" s="32">
@@ -4628,7 +4681,7 @@
       <c r="H6" s="32">
         <v>600</v>
       </c>
-      <c r="I6" s="32">
+      <c r="I6" s="36">
         <v>5</v>
       </c>
       <c r="J6" s="32">
@@ -4685,7 +4738,7 @@
       <c r="AA6" s="32">
         <v>600</v>
       </c>
-      <c r="AB6" s="32">
+      <c r="AB6" s="36">
         <v>79</v>
       </c>
       <c r="AC6" s="32">
@@ -4756,7 +4809,7 @@
       <c r="B7" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="42">
         <v>7</v>
       </c>
       <c r="D7" s="32">
@@ -4774,8 +4827,8 @@
       <c r="H7" s="32">
         <v>600</v>
       </c>
-      <c r="I7" s="32">
-        <v>5</v>
+      <c r="I7" s="41" t="s">
+        <v>193</v>
       </c>
       <c r="J7" s="32">
         <v>600</v>
@@ -4831,7 +4884,7 @@
       <c r="AA7" s="32">
         <v>600</v>
       </c>
-      <c r="AB7" s="32">
+      <c r="AB7" s="36">
         <v>7</v>
       </c>
       <c r="AC7" s="32">
@@ -4902,7 +4955,7 @@
       <c r="B8" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="36">
         <v>3</v>
       </c>
       <c r="D8" s="32">
@@ -4977,7 +5030,7 @@
       <c r="AA8" s="32">
         <v>600</v>
       </c>
-      <c r="AB8" s="32">
+      <c r="AB8" s="36">
         <v>9</v>
       </c>
       <c r="AC8" s="32">
@@ -5126,16 +5179,16 @@
       <c r="AB9" s="32">
         <v>600</v>
       </c>
-      <c r="AC9" s="32">
+      <c r="AC9" s="43">
         <v>10</v>
       </c>
-      <c r="AD9" s="32">
+      <c r="AD9" s="43">
         <v>11</v>
       </c>
-      <c r="AE9" s="32">
+      <c r="AE9" s="43">
         <v>12</v>
       </c>
-      <c r="AF9" s="32">
+      <c r="AF9" s="43">
         <v>13</v>
       </c>
       <c r="AG9" s="32">
@@ -5194,7 +5247,7 @@
       <c r="B10" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="36">
         <v>15</v>
       </c>
       <c r="D10" s="32">
@@ -5263,10 +5316,10 @@
       <c r="Y10" s="32">
         <v>600</v>
       </c>
-      <c r="Z10" s="32">
+      <c r="Z10" s="36">
         <v>15</v>
       </c>
-      <c r="AA10" s="32">
+      <c r="AA10" s="36">
         <v>1</v>
       </c>
       <c r="AB10" s="32">
@@ -5299,34 +5352,34 @@
       <c r="AK10" s="32">
         <v>600</v>
       </c>
-      <c r="AL10" s="32">
+      <c r="AL10" s="36">
         <v>15</v>
       </c>
-      <c r="AM10" s="32">
+      <c r="AM10" s="36">
         <v>15</v>
       </c>
-      <c r="AN10" s="32">
+      <c r="AN10" s="36">
         <v>15</v>
       </c>
-      <c r="AO10" s="32">
+      <c r="AO10" s="36">
         <v>15</v>
       </c>
-      <c r="AP10" s="32">
+      <c r="AP10" s="36">
         <v>15</v>
       </c>
-      <c r="AQ10" s="32">
+      <c r="AQ10" s="36">
         <v>15</v>
       </c>
-      <c r="AR10" s="32">
+      <c r="AR10" s="36">
         <v>15</v>
       </c>
       <c r="AS10" s="32">
         <v>600</v>
       </c>
-      <c r="AT10" s="32">
+      <c r="AT10" s="36">
         <v>15</v>
       </c>
-      <c r="AU10" s="32">
+      <c r="AU10" s="36">
         <v>15</v>
       </c>
       <c r="AV10" s="32">
@@ -5340,7 +5393,7 @@
       <c r="B11" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="36">
         <v>18</v>
       </c>
       <c r="D11" s="32">
@@ -5409,7 +5462,7 @@
       <c r="Y11" s="32">
         <v>600</v>
       </c>
-      <c r="Z11" s="32">
+      <c r="Z11" s="36">
         <v>17</v>
       </c>
       <c r="AA11" s="32">
@@ -5445,34 +5498,34 @@
       <c r="AK11" s="32">
         <v>600</v>
       </c>
-      <c r="AL11" s="32">
+      <c r="AL11" s="43">
         <v>19</v>
       </c>
-      <c r="AM11" s="32">
+      <c r="AM11" s="36">
         <v>17</v>
       </c>
-      <c r="AN11" s="32">
+      <c r="AN11" s="36">
         <v>17</v>
       </c>
-      <c r="AO11" s="32">
+      <c r="AO11" s="43">
         <v>20</v>
       </c>
-      <c r="AP11" s="32">
+      <c r="AP11" s="36">
         <v>17</v>
       </c>
-      <c r="AQ11" s="32">
+      <c r="AQ11" s="43">
         <v>21</v>
       </c>
-      <c r="AR11" s="32">
+      <c r="AR11" s="36">
         <v>17</v>
       </c>
       <c r="AS11" s="32">
         <v>600</v>
       </c>
-      <c r="AT11" s="32">
+      <c r="AT11" s="43">
         <v>22</v>
       </c>
-      <c r="AU11" s="32">
+      <c r="AU11" s="43">
         <v>23</v>
       </c>
       <c r="AV11" s="32">
@@ -5486,7 +5539,7 @@
       <c r="B12" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="36">
         <v>26</v>
       </c>
       <c r="D12" s="32">
@@ -5591,7 +5644,7 @@
       <c r="AK12" s="32">
         <v>600</v>
       </c>
-      <c r="AL12" s="32">
+      <c r="AL12" s="36">
         <v>32</v>
       </c>
       <c r="AM12" s="32">
@@ -5600,13 +5653,13 @@
       <c r="AN12" s="32">
         <v>600</v>
       </c>
-      <c r="AO12" s="32">
+      <c r="AO12" s="36">
         <v>35</v>
       </c>
       <c r="AP12" s="32">
         <v>600</v>
       </c>
-      <c r="AQ12" s="32">
+      <c r="AQ12" s="36">
         <v>36</v>
       </c>
       <c r="AR12" s="32">
@@ -5615,10 +5668,10 @@
       <c r="AS12" s="32">
         <v>600</v>
       </c>
-      <c r="AT12" s="32">
+      <c r="AT12" s="36">
         <v>37</v>
       </c>
-      <c r="AU12" s="32">
+      <c r="AU12" s="36">
         <v>41</v>
       </c>
       <c r="AV12" s="32">
@@ -5632,7 +5685,7 @@
       <c r="B13" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="C13" s="32">
+      <c r="C13" s="36">
         <v>16</v>
       </c>
       <c r="D13" s="32">
@@ -5701,7 +5754,7 @@
       <c r="Y13" s="32">
         <v>600</v>
       </c>
-      <c r="Z13" s="32">
+      <c r="Z13" s="36">
         <v>25</v>
       </c>
       <c r="AA13" s="32">
@@ -5737,34 +5790,34 @@
       <c r="AK13" s="32">
         <v>600</v>
       </c>
-      <c r="AL13" s="32">
+      <c r="AL13" s="36">
         <v>16</v>
       </c>
-      <c r="AM13" s="32">
+      <c r="AM13" s="36">
         <v>25</v>
       </c>
-      <c r="AN13" s="32">
+      <c r="AN13" s="36">
         <v>25</v>
       </c>
-      <c r="AO13" s="32">
+      <c r="AO13" s="36">
         <v>16</v>
       </c>
-      <c r="AP13" s="32">
+      <c r="AP13" s="36">
         <v>25</v>
       </c>
-      <c r="AQ13" s="32">
+      <c r="AQ13" s="36">
         <v>16</v>
       </c>
-      <c r="AR13" s="32">
+      <c r="AR13" s="36">
         <v>25</v>
       </c>
       <c r="AS13" s="32">
         <v>600</v>
       </c>
-      <c r="AT13" s="32">
+      <c r="AT13" s="36">
         <v>16</v>
       </c>
-      <c r="AU13" s="32">
+      <c r="AU13" s="36">
         <v>16</v>
       </c>
       <c r="AV13" s="32">
@@ -5778,7 +5831,7 @@
       <c r="B14" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="36">
         <v>27</v>
       </c>
       <c r="D14" s="32">
@@ -5924,7 +5977,7 @@
       <c r="B15" s="31" t="s">
         <v>171</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="36">
         <v>27</v>
       </c>
       <c r="D15" s="32">
@@ -6073,7 +6126,7 @@
       <c r="C16" s="32">
         <v>600</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="36">
         <v>29</v>
       </c>
       <c r="E16" s="32">
@@ -6088,7 +6141,7 @@
       <c r="H16" s="32">
         <v>600</v>
       </c>
-      <c r="I16" s="32">
+      <c r="I16" s="36">
         <v>28</v>
       </c>
       <c r="J16" s="32">
@@ -6222,7 +6275,7 @@
       <c r="D17" s="32">
         <v>600</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="36">
         <v>30</v>
       </c>
       <c r="F17" s="32">
@@ -6237,7 +6290,7 @@
       <c r="I17" s="32">
         <v>600</v>
       </c>
-      <c r="J17" s="32">
+      <c r="J17" s="36">
         <v>31</v>
       </c>
       <c r="K17" s="32">
@@ -6467,7 +6520,7 @@
       <c r="AK18" s="32">
         <v>600</v>
       </c>
-      <c r="AL18" s="32">
+      <c r="AL18" s="36">
         <v>32</v>
       </c>
       <c r="AM18" s="32">
@@ -6616,10 +6669,10 @@
       <c r="AL19" s="32">
         <v>600</v>
       </c>
-      <c r="AM19" s="32">
+      <c r="AM19" s="36">
         <v>33</v>
       </c>
-      <c r="AN19" s="32">
+      <c r="AN19" s="36">
         <v>34</v>
       </c>
       <c r="AO19" s="32">
@@ -6768,7 +6821,7 @@
       <c r="AN20" s="32">
         <v>600</v>
       </c>
-      <c r="AO20" s="32">
+      <c r="AO20" s="36">
         <v>35</v>
       </c>
       <c r="AP20" s="32">
@@ -6920,7 +6973,7 @@
       <c r="AP21" s="32">
         <v>600</v>
       </c>
-      <c r="AQ21" s="32">
+      <c r="AQ21" s="36">
         <v>36</v>
       </c>
       <c r="AR21" s="32">
@@ -7075,7 +7128,7 @@
       <c r="AS22" s="32">
         <v>600</v>
       </c>
-      <c r="AT22" s="32">
+      <c r="AT22" s="36">
         <v>37</v>
       </c>
       <c r="AU22" s="32">
@@ -7092,7 +7145,7 @@
       <c r="B23" s="31" t="s">
         <v>179</v>
       </c>
-      <c r="C23" s="32">
+      <c r="C23" s="36">
         <v>38</v>
       </c>
       <c r="D23" s="32">
@@ -7244,7 +7297,7 @@
       <c r="D24" s="32">
         <v>600</v>
       </c>
-      <c r="E24" s="32">
+      <c r="E24" s="36">
         <v>39</v>
       </c>
       <c r="F24" s="32">
@@ -7253,7 +7306,7 @@
       <c r="G24" s="32">
         <v>600</v>
       </c>
-      <c r="H24" s="32">
+      <c r="H24" s="36">
         <v>40</v>
       </c>
       <c r="I24" s="32">
@@ -7516,7 +7569,7 @@
       <c r="AT25" s="32">
         <v>600</v>
       </c>
-      <c r="AU25" s="32">
+      <c r="AU25" s="36">
         <v>41</v>
       </c>
       <c r="AV25" s="32">
@@ -7530,7 +7583,7 @@
       <c r="B26" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="C26" s="32">
+      <c r="C26" s="36">
         <v>45</v>
       </c>
       <c r="D26" s="32">
@@ -7542,7 +7595,7 @@
       <c r="F26" s="32">
         <v>600</v>
       </c>
-      <c r="G26" s="32">
+      <c r="G26" s="36">
         <v>45</v>
       </c>
       <c r="H26" s="32">
@@ -7593,7 +7646,7 @@
       <c r="W26" s="32">
         <v>600</v>
       </c>
-      <c r="X26" s="32">
+      <c r="X26" s="36">
         <v>45</v>
       </c>
       <c r="Y26" s="32">
@@ -7620,19 +7673,19 @@
       <c r="AF26" s="32">
         <v>600</v>
       </c>
-      <c r="AG26" s="32">
+      <c r="AG26" s="36">
         <v>45</v>
       </c>
-      <c r="AH26" s="32">
+      <c r="AH26" s="36">
         <v>45</v>
       </c>
-      <c r="AI26" s="32">
+      <c r="AI26" s="36">
         <v>45</v>
       </c>
-      <c r="AJ26" s="32">
+      <c r="AJ26" s="36">
         <v>45</v>
       </c>
-      <c r="AK26" s="32">
+      <c r="AK26" s="36">
         <v>45</v>
       </c>
       <c r="AL26" s="32">
@@ -7682,7 +7735,7 @@
       <c r="D27" s="32">
         <v>600</v>
       </c>
-      <c r="E27" s="32">
+      <c r="E27" s="36">
         <v>43</v>
       </c>
       <c r="F27" s="32">
@@ -7691,7 +7744,7 @@
       <c r="G27" s="32">
         <v>600</v>
       </c>
-      <c r="H27" s="32">
+      <c r="H27" s="36">
         <v>44</v>
       </c>
       <c r="I27" s="32">
@@ -7828,22 +7881,22 @@
       <c r="D28" s="32">
         <v>600</v>
       </c>
-      <c r="E28" s="32">
+      <c r="E28" s="36">
         <v>48</v>
       </c>
-      <c r="F28" s="32">
+      <c r="F28" s="36">
         <v>48</v>
       </c>
       <c r="G28" s="32">
         <v>600</v>
       </c>
-      <c r="H28" s="32">
+      <c r="H28" s="36">
         <v>48</v>
       </c>
       <c r="I28" s="32">
         <v>600</v>
       </c>
-      <c r="J28" s="32">
+      <c r="J28" s="36">
         <v>48</v>
       </c>
       <c r="K28" s="32">
@@ -7974,22 +8027,22 @@
       <c r="D29" s="32">
         <v>600</v>
       </c>
-      <c r="E29" s="32">
+      <c r="E29" s="36">
         <v>47</v>
       </c>
-      <c r="F29" s="32">
+      <c r="F29" s="36">
         <v>47</v>
       </c>
       <c r="G29" s="32">
         <v>600</v>
       </c>
-      <c r="H29" s="32">
+      <c r="H29" s="36">
         <v>47</v>
       </c>
       <c r="I29" s="32">
         <v>600</v>
       </c>
-      <c r="J29" s="32">
+      <c r="J29" s="36">
         <v>47</v>
       </c>
       <c r="K29" s="32">
@@ -8025,7 +8078,7 @@
       <c r="U29" s="32">
         <v>600</v>
       </c>
-      <c r="V29" s="32">
+      <c r="V29" s="36">
         <v>46</v>
       </c>
       <c r="W29" s="32">
@@ -8120,22 +8173,22 @@
       <c r="D30" s="32">
         <v>600</v>
       </c>
-      <c r="E30" s="32">
+      <c r="E30" s="36">
         <v>51</v>
       </c>
-      <c r="F30" s="32">
+      <c r="F30" s="36">
         <v>51</v>
       </c>
       <c r="G30" s="32">
         <v>600</v>
       </c>
-      <c r="H30" s="32">
+      <c r="H30" s="36">
         <v>51</v>
       </c>
       <c r="I30" s="32">
         <v>600</v>
       </c>
-      <c r="J30" s="32">
+      <c r="J30" s="36">
         <v>51</v>
       </c>
       <c r="K30" s="32">
@@ -8171,7 +8224,7 @@
       <c r="U30" s="32">
         <v>600</v>
       </c>
-      <c r="V30" s="32">
+      <c r="V30" s="36">
         <v>51</v>
       </c>
       <c r="W30" s="32">
@@ -8266,22 +8319,22 @@
       <c r="D31" s="32">
         <v>600</v>
       </c>
-      <c r="E31" s="32">
+      <c r="E31" s="36">
         <v>50</v>
       </c>
-      <c r="F31" s="32">
+      <c r="F31" s="36">
         <v>50</v>
       </c>
       <c r="G31" s="32">
         <v>600</v>
       </c>
-      <c r="H31" s="32">
+      <c r="H31" s="36">
         <v>50</v>
       </c>
       <c r="I31" s="32">
         <v>600</v>
       </c>
-      <c r="J31" s="32">
+      <c r="J31" s="36">
         <v>50</v>
       </c>
       <c r="K31" s="32">
@@ -8317,10 +8370,10 @@
       <c r="U31" s="32">
         <v>600</v>
       </c>
-      <c r="V31" s="32">
+      <c r="V31" s="36">
         <v>50</v>
       </c>
-      <c r="W31" s="32">
+      <c r="W31" s="36">
         <v>49</v>
       </c>
       <c r="X31" s="32">
@@ -8403,145 +8456,145 @@
       <c r="A32" s="33">
         <v>30</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="44" t="s">
         <v>184</v>
       </c>
-      <c r="C32" s="32">
-        <v>600</v>
-      </c>
-      <c r="D32" s="32">
-        <v>600</v>
-      </c>
-      <c r="E32" s="32">
-        <v>600</v>
-      </c>
-      <c r="F32" s="32">
-        <v>600</v>
-      </c>
-      <c r="G32" s="32">
-        <v>600</v>
-      </c>
-      <c r="H32" s="32">
-        <v>600</v>
-      </c>
-      <c r="I32" s="32">
-        <v>600</v>
-      </c>
-      <c r="J32" s="32">
-        <v>600</v>
-      </c>
-      <c r="K32" s="32">
-        <v>600</v>
-      </c>
-      <c r="L32" s="32">
-        <v>600</v>
-      </c>
-      <c r="M32" s="32">
-        <v>600</v>
-      </c>
-      <c r="N32" s="32">
-        <v>600</v>
-      </c>
-      <c r="O32" s="32">
-        <v>600</v>
-      </c>
-      <c r="P32" s="32">
-        <v>600</v>
-      </c>
-      <c r="Q32" s="32">
-        <v>600</v>
-      </c>
-      <c r="R32" s="32">
-        <v>600</v>
-      </c>
-      <c r="S32" s="32">
-        <v>600</v>
-      </c>
-      <c r="T32" s="32">
-        <v>600</v>
-      </c>
-      <c r="U32" s="32">
-        <v>600</v>
-      </c>
-      <c r="V32" s="32">
-        <v>600</v>
-      </c>
-      <c r="W32" s="32">
-        <v>600</v>
-      </c>
-      <c r="X32" s="32">
-        <v>51</v>
-      </c>
-      <c r="Y32" s="32">
-        <v>600</v>
-      </c>
-      <c r="Z32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AA32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AB32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AC32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AD32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AE32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AF32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AG32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AH32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AI32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AJ32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AK32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AL32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AM32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AN32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AO32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AP32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AQ32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AR32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AS32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AT32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AU32" s="32">
-        <v>600</v>
-      </c>
-      <c r="AV32" s="32">
+      <c r="C32" s="40">
+        <v>600</v>
+      </c>
+      <c r="D32" s="40">
+        <v>600</v>
+      </c>
+      <c r="E32" s="40">
+        <v>600</v>
+      </c>
+      <c r="F32" s="40">
+        <v>600</v>
+      </c>
+      <c r="G32" s="40">
+        <v>600</v>
+      </c>
+      <c r="H32" s="40">
+        <v>600</v>
+      </c>
+      <c r="I32" s="40">
+        <v>600</v>
+      </c>
+      <c r="J32" s="40">
+        <v>600</v>
+      </c>
+      <c r="K32" s="40">
+        <v>600</v>
+      </c>
+      <c r="L32" s="40">
+        <v>600</v>
+      </c>
+      <c r="M32" s="40">
+        <v>600</v>
+      </c>
+      <c r="N32" s="40">
+        <v>600</v>
+      </c>
+      <c r="O32" s="40">
+        <v>600</v>
+      </c>
+      <c r="P32" s="40">
+        <v>600</v>
+      </c>
+      <c r="Q32" s="40">
+        <v>600</v>
+      </c>
+      <c r="R32" s="40">
+        <v>600</v>
+      </c>
+      <c r="S32" s="40">
+        <v>600</v>
+      </c>
+      <c r="T32" s="40">
+        <v>600</v>
+      </c>
+      <c r="U32" s="40">
+        <v>600</v>
+      </c>
+      <c r="V32" s="40">
+        <v>600</v>
+      </c>
+      <c r="W32" s="40">
+        <v>600</v>
+      </c>
+      <c r="X32" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y32" s="40">
+        <v>600</v>
+      </c>
+      <c r="Z32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AA32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AB32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AC32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AD32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AE32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AF32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AG32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AH32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AI32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AJ32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AK32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AL32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AM32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AN32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AO32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AP32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AQ32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AR32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AS32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AT32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AU32" s="40">
+        <v>600</v>
+      </c>
+      <c r="AV32" s="40">
         <v>600</v>
       </c>
     </row>
@@ -8552,7 +8605,7 @@
       <c r="B33" s="31" t="s">
         <v>185</v>
       </c>
-      <c r="C33" s="32">
+      <c r="C33" s="36">
         <v>53</v>
       </c>
       <c r="D33" s="32">
@@ -8564,7 +8617,7 @@
       <c r="F33" s="32">
         <v>600</v>
       </c>
-      <c r="G33" s="32">
+      <c r="G33" s="36">
         <v>53</v>
       </c>
       <c r="H33" s="32">
@@ -8615,7 +8668,7 @@
       <c r="W33" s="32">
         <v>600</v>
       </c>
-      <c r="X33" s="32">
+      <c r="X33" s="36">
         <v>52</v>
       </c>
       <c r="Y33" s="32">
@@ -8642,19 +8695,19 @@
       <c r="AF33" s="32">
         <v>600</v>
       </c>
-      <c r="AG33" s="32">
+      <c r="AG33" s="36">
         <v>53</v>
       </c>
-      <c r="AH33" s="32">
+      <c r="AH33" s="36">
         <v>53</v>
       </c>
-      <c r="AI33" s="32">
+      <c r="AI33" s="36">
         <v>53</v>
       </c>
-      <c r="AJ33" s="32">
+      <c r="AJ33" s="36">
         <v>53</v>
       </c>
-      <c r="AK33" s="32">
+      <c r="AK33" s="36">
         <v>53</v>
       </c>
       <c r="AL33" s="32">
@@ -8698,7 +8751,7 @@
       <c r="B34" s="31" t="s">
         <v>186</v>
       </c>
-      <c r="C34" s="32">
+      <c r="C34" s="36">
         <v>63</v>
       </c>
       <c r="D34" s="32">
@@ -8710,7 +8763,7 @@
       <c r="F34" s="32">
         <v>600</v>
       </c>
-      <c r="G34" s="32">
+      <c r="G34" s="36">
         <v>63</v>
       </c>
       <c r="H34" s="32">
@@ -8788,19 +8841,19 @@
       <c r="AF34" s="32">
         <v>600</v>
       </c>
-      <c r="AG34" s="32">
+      <c r="AG34" s="36">
         <v>63</v>
       </c>
-      <c r="AH34" s="32">
+      <c r="AH34" s="36">
         <v>63</v>
       </c>
-      <c r="AI34" s="32">
+      <c r="AI34" s="36">
         <v>63</v>
       </c>
-      <c r="AJ34" s="32">
+      <c r="AJ34" s="36">
         <v>63</v>
       </c>
-      <c r="AK34" s="32">
+      <c r="AK34" s="36">
         <v>63</v>
       </c>
       <c r="AL34" s="32">
@@ -8850,22 +8903,22 @@
       <c r="D35" s="32">
         <v>600</v>
       </c>
-      <c r="E35" s="32">
+      <c r="E35" s="36">
         <v>56</v>
       </c>
-      <c r="F35" s="32">
+      <c r="F35" s="36">
         <v>56</v>
       </c>
       <c r="G35" s="32">
         <v>600</v>
       </c>
-      <c r="H35" s="32">
+      <c r="H35" s="36">
         <v>56</v>
       </c>
       <c r="I35" s="32">
         <v>600</v>
       </c>
-      <c r="J35" s="32">
+      <c r="J35" s="36">
         <v>56</v>
       </c>
       <c r="K35" s="32">
@@ -8883,28 +8936,28 @@
       <c r="O35" s="32">
         <v>600</v>
       </c>
-      <c r="P35" s="32">
+      <c r="P35" s="43">
         <v>57</v>
       </c>
-      <c r="Q35" s="32">
+      <c r="Q35" s="43">
         <v>59</v>
       </c>
-      <c r="R35" s="32">
+      <c r="R35" s="43">
         <v>61</v>
       </c>
-      <c r="S35" s="32">
+      <c r="S35" s="43">
         <v>60</v>
       </c>
-      <c r="T35" s="32">
+      <c r="T35" s="43">
         <v>62</v>
       </c>
-      <c r="U35" s="32">
+      <c r="U35" s="43">
         <v>58</v>
       </c>
-      <c r="V35" s="32">
+      <c r="V35" s="36">
         <v>56</v>
       </c>
-      <c r="W35" s="32">
+      <c r="W35" s="36">
         <v>56</v>
       </c>
       <c r="X35" s="32">
@@ -9029,29 +9082,29 @@
       <c r="O36" s="32">
         <v>600</v>
       </c>
-      <c r="P36" s="32">
+      <c r="P36" s="36">
         <v>57</v>
       </c>
-      <c r="Q36" s="32">
+      <c r="Q36" s="36">
         <v>59</v>
       </c>
-      <c r="R36" s="32">
+      <c r="R36" s="36">
         <v>61</v>
       </c>
-      <c r="S36" s="32">
+      <c r="S36" s="36">
         <v>60</v>
       </c>
-      <c r="T36" s="32">
+      <c r="T36" s="36">
         <v>62</v>
       </c>
-      <c r="U36" s="32">
+      <c r="U36" s="36">
         <v>58</v>
       </c>
-      <c r="V36" s="32">
-        <v>56</v>
-      </c>
-      <c r="W36" s="32">
-        <v>56</v>
+      <c r="V36" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="W36" s="41" t="s">
+        <v>195</v>
       </c>
       <c r="X36" s="32">
         <v>600</v>
@@ -9136,7 +9189,7 @@
       <c r="B37" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="C37" s="32">
+      <c r="C37" s="36">
         <v>67</v>
       </c>
       <c r="D37" s="32">
@@ -9148,7 +9201,7 @@
       <c r="F37" s="32">
         <v>600</v>
       </c>
-      <c r="G37" s="32">
+      <c r="G37" s="36">
         <v>67</v>
       </c>
       <c r="H37" s="32">
@@ -9226,19 +9279,19 @@
       <c r="AF37" s="32">
         <v>600</v>
       </c>
-      <c r="AG37" s="32">
+      <c r="AG37" s="36">
         <v>67</v>
       </c>
-      <c r="AH37" s="32">
+      <c r="AH37" s="36">
         <v>67</v>
       </c>
-      <c r="AI37" s="32">
+      <c r="AI37" s="36">
         <v>67</v>
       </c>
-      <c r="AJ37" s="32">
+      <c r="AJ37" s="36">
         <v>67</v>
       </c>
-      <c r="AK37" s="32">
+      <c r="AK37" s="36">
         <v>67</v>
       </c>
       <c r="AL37" s="32">
@@ -9288,28 +9341,28 @@
       <c r="D38" s="32">
         <v>600</v>
       </c>
-      <c r="E38" s="32">
+      <c r="E38" s="36">
         <v>66</v>
       </c>
-      <c r="F38" s="32">
+      <c r="F38" s="36">
         <v>66</v>
       </c>
       <c r="G38" s="32">
         <v>600</v>
       </c>
-      <c r="H38" s="32">
+      <c r="H38" s="36">
         <v>66</v>
       </c>
       <c r="I38" s="32">
         <v>600</v>
       </c>
-      <c r="J38" s="32">
+      <c r="J38" s="36">
         <v>66</v>
       </c>
-      <c r="K38" s="32">
+      <c r="K38" s="36">
         <v>64</v>
       </c>
-      <c r="L38" s="32">
+      <c r="L38" s="36">
         <v>65</v>
       </c>
       <c r="M38" s="32">
@@ -9321,28 +9374,28 @@
       <c r="O38" s="32">
         <v>600</v>
       </c>
-      <c r="P38" s="32">
+      <c r="P38" s="36">
         <v>66</v>
       </c>
-      <c r="Q38" s="32">
+      <c r="Q38" s="36">
         <v>66</v>
       </c>
-      <c r="R38" s="32">
+      <c r="R38" s="36">
         <v>66</v>
       </c>
-      <c r="S38" s="32">
+      <c r="S38" s="36">
         <v>66</v>
       </c>
-      <c r="T38" s="32">
+      <c r="T38" s="36">
         <v>66</v>
       </c>
-      <c r="U38" s="32">
+      <c r="U38" s="36">
         <v>66</v>
       </c>
-      <c r="V38" s="32">
+      <c r="V38" s="36">
         <v>66</v>
       </c>
-      <c r="W38" s="32">
+      <c r="W38" s="36">
         <v>66</v>
       </c>
       <c r="X38" s="32">
@@ -9428,7 +9481,7 @@
       <c r="B39" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="C39" s="32">
+      <c r="C39" s="36">
         <v>72</v>
       </c>
       <c r="D39" s="32">
@@ -9440,7 +9493,7 @@
       <c r="F39" s="32">
         <v>600</v>
       </c>
-      <c r="G39" s="32">
+      <c r="G39" s="36">
         <v>72</v>
       </c>
       <c r="H39" s="32">
@@ -9518,19 +9571,19 @@
       <c r="AF39" s="32">
         <v>600</v>
       </c>
-      <c r="AG39" s="32">
+      <c r="AG39" s="36">
         <v>72</v>
       </c>
-      <c r="AH39" s="32">
+      <c r="AH39" s="36">
         <v>72</v>
       </c>
-      <c r="AI39" s="32">
+      <c r="AI39" s="36">
         <v>72</v>
       </c>
-      <c r="AJ39" s="32">
+      <c r="AJ39" s="36">
         <v>72</v>
       </c>
-      <c r="AK39" s="32">
+      <c r="AK39" s="36">
         <v>72</v>
       </c>
       <c r="AL39" s="32">
@@ -9580,61 +9633,61 @@
       <c r="D40" s="32">
         <v>600</v>
       </c>
-      <c r="E40" s="32">
+      <c r="E40" s="36">
         <v>71</v>
       </c>
-      <c r="F40" s="32">
+      <c r="F40" s="36">
         <v>71</v>
       </c>
       <c r="G40" s="32">
         <v>600</v>
       </c>
-      <c r="H40" s="32">
+      <c r="H40" s="36">
         <v>71</v>
       </c>
       <c r="I40" s="32">
         <v>600</v>
       </c>
-      <c r="J40" s="32">
+      <c r="J40" s="36">
         <v>71</v>
       </c>
-      <c r="K40" s="32">
+      <c r="K40" s="36">
         <v>71</v>
       </c>
-      <c r="L40" s="32">
+      <c r="L40" s="36">
         <v>71</v>
       </c>
-      <c r="M40" s="32">
+      <c r="M40" s="36">
         <v>68</v>
       </c>
-      <c r="N40" s="32">
+      <c r="N40" s="36">
         <v>69</v>
       </c>
-      <c r="O40" s="32">
+      <c r="O40" s="36">
         <v>70</v>
       </c>
-      <c r="P40" s="32">
+      <c r="P40" s="36">
         <v>71</v>
       </c>
-      <c r="Q40" s="32">
+      <c r="Q40" s="36">
         <v>71</v>
       </c>
-      <c r="R40" s="32">
+      <c r="R40" s="36">
         <v>71</v>
       </c>
-      <c r="S40" s="32">
+      <c r="S40" s="36">
         <v>71</v>
       </c>
-      <c r="T40" s="32">
+      <c r="T40" s="36">
         <v>71</v>
       </c>
-      <c r="U40" s="32">
+      <c r="U40" s="36">
         <v>71</v>
       </c>
-      <c r="V40" s="32">
+      <c r="V40" s="36">
         <v>71</v>
       </c>
-      <c r="W40" s="32">
+      <c r="W40" s="36">
         <v>71</v>
       </c>
       <c r="X40" s="32">
@@ -9720,7 +9773,7 @@
       <c r="B41" s="31" t="s">
         <v>191</v>
       </c>
-      <c r="C41" s="32">
+      <c r="C41" s="36">
         <v>27</v>
       </c>
       <c r="D41" s="32">
@@ -9732,7 +9785,7 @@
       <c r="F41" s="32">
         <v>600</v>
       </c>
-      <c r="G41" s="32">
+      <c r="G41" s="36">
         <v>78</v>
       </c>
       <c r="H41" s="32">
@@ -9810,19 +9863,19 @@
       <c r="AF41" s="32">
         <v>600</v>
       </c>
-      <c r="AG41" s="32">
+      <c r="AG41" s="36">
         <v>73</v>
       </c>
-      <c r="AH41" s="32">
+      <c r="AH41" s="36">
         <v>74</v>
       </c>
-      <c r="AI41" s="32">
+      <c r="AI41" s="36">
         <v>75</v>
       </c>
-      <c r="AJ41" s="32">
+      <c r="AJ41" s="36">
         <v>76</v>
       </c>
-      <c r="AK41" s="32">
+      <c r="AK41" s="36">
         <v>77</v>
       </c>
       <c r="AL41" s="32">
@@ -12222,7 +12275,7 @@
   <dimension ref="A1:AP46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3"/>
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>